<commit_message>
write the profile file in a excel
</commit_message>
<xml_diff>
--- a/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
+++ b/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ti\simplelink\ble_cc26xx_2_01_01_44627_copy\SimpleBLEPeripheral\protocol\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24150" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="simple BLE peripheral" sheetId="1" r:id="rId1"/>
@@ -769,7 +764,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -899,6 +894,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1028,24 +1036,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1056,53 +1055,71 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1372,7 +1389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1380,37 +1397,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="58.5" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1420,104 +1437,108 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="9">
         <v>1.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="12">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -1527,11 +1548,12 @@
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="9">
         <v>5.4166666666666669E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1544,532 +1566,558 @@
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
+    <row r="19" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="8" t="s">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="8">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
+    <row r="32" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="8" t="s">
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="8">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E37" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="8" t="s">
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E40" t="s">
+      <c r="D40" s="8"/>
+      <c r="E40" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="8" t="s">
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E44" t="s">
+      <c r="D44" s="8"/>
+      <c r="E44" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="8" t="s">
         <v>129</v>
       </c>
+      <c r="E45" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
write a new profile charicteristic
</commit_message>
<xml_diff>
--- a/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
+++ b/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="simple BLE peripheral" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="141">
   <si>
     <t>Handle</t>
   </si>
@@ -297,118 +298,176 @@
     <t xml:space="preserve">    Simple Profile Char 1</t>
   </si>
   <si>
+    <t>0x001F</t>
+  </si>
+  <si>
+    <t>0x2901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Characteristic User Description</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>02:21:00:F2:FF</t>
+  </si>
+  <si>
+    <t>0x0021</t>
+  </si>
+  <si>
+    <t>0xFFF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 2</t>
+  </si>
+  <si>
+    <t>0x0022</t>
+  </si>
+  <si>
+    <t>0x0023</t>
+  </si>
+  <si>
+    <t>08:24:00:F3:FF</t>
+  </si>
+  <si>
+    <t>0x0024</t>
+  </si>
+  <si>
+    <t>0xFFF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 3</t>
+  </si>
+  <si>
+    <t>0x0025</t>
+  </si>
+  <si>
+    <t>0x0026</t>
+  </si>
+  <si>
+    <t>10:27:00:F4:FF</t>
+  </si>
+  <si>
+    <t>0x0027</t>
+  </si>
+  <si>
+    <t>0xFFF4</t>
+  </si>
+  <si>
+    <t>Nfy  0x10</t>
+  </si>
+  <si>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x2902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Client Characteristic Configuration</t>
+  </si>
+  <si>
+    <t>0x0029</t>
+  </si>
+  <si>
+    <t>start flag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transducer_Driver_Parameter</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>Rd Wr  0x0A</t>
-  </si>
-  <si>
-    <t>0x001F</t>
-  </si>
-  <si>
-    <t>0x2901</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rd Wr  0x0A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">    Characteristic User Description</t>
-  </si>
-  <si>
-    <t>Characteristic 1</t>
-  </si>
-  <si>
-    <t>0x0020</t>
-  </si>
-  <si>
-    <t>02:21:00:F2:FF</t>
-  </si>
-  <si>
-    <t>0x0021</t>
-  </si>
-  <si>
-    <t>0xFFF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Simple Profile Char 2</t>
-  </si>
-  <si>
-    <t>0x0022</t>
-  </si>
-  <si>
-    <t>Characteristic 2</t>
-  </si>
-  <si>
-    <t>0x0023</t>
-  </si>
-  <si>
-    <t>08:24:00:F3:FF</t>
-  </si>
-  <si>
-    <t>0x0024</t>
-  </si>
-  <si>
-    <t>0xFFF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Simple Profile Char 3</t>
-  </si>
-  <si>
-    <t>Wr  0x08</t>
-  </si>
-  <si>
-    <t>0x0025</t>
-  </si>
-  <si>
-    <t>Characteristic 3</t>
-  </si>
-  <si>
-    <t>0x0026</t>
-  </si>
-  <si>
-    <t>10:27:00:F4:FF</t>
-  </si>
-  <si>
-    <t>0x0027</t>
-  </si>
-  <si>
-    <t>0xFFF4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter 1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter 2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00:00</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIFO date</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 byte max</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>total 768</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIFO row</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">48 row </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>data ready</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">    Simple Profile Char 4</t>
-  </si>
-  <si>
-    <t>Nfy  0x10</t>
-  </si>
-  <si>
-    <t>0x0028</t>
-  </si>
-  <si>
-    <t>0x2902</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Client Characteristic Configuration</t>
-  </si>
-  <si>
-    <t>0x0029</t>
-  </si>
-  <si>
-    <t>Characteristic 4</t>
-  </si>
-  <si>
-    <t>0x002A</t>
-  </si>
-  <si>
-    <t>02:2B:00:F5:FF</t>
-  </si>
-  <si>
-    <t>0x002B</t>
-  </si>
-  <si>
-    <t>0xFFF5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">    Simple Profile Char 5</t>
-  </si>
-  <si>
-    <t>0x002C</t>
-  </si>
-  <si>
-    <t>Characteristic 5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGA450_Parameter</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>48 row</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notify the current row of data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1115,6 +1174,130 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4390309</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>114015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="8467725"/>
+          <a:ext cx="5723809" cy="2276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4448175</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>65855</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5819775" y="8420100"/>
+          <a:ext cx="6561905" cy="1485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>532390</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>37152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8076190" cy="7580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1380,16 +1563,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="58.5" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1638,7 +1821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>49</v>
       </c>
@@ -1652,7 +1835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1669,7 +1852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>55</v>
       </c>
@@ -1683,7 +1866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1700,7 +1883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
         <v>61</v>
       </c>
@@ -1714,7 +1897,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1731,7 +1914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>67</v>
       </c>
@@ -1745,7 +1928,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1762,7 +1945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
         <v>73</v>
       </c>
@@ -1776,7 +1959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1793,7 +1976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
         <v>79</v>
       </c>
@@ -1807,7 +1990,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1824,7 +2007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
         <v>85</v>
       </c>
@@ -1838,7 +2021,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
         <v>87</v>
       </c>
@@ -1851,8 +2034,11 @@
       <c r="D30" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F30" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -1866,26 +2052,26 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>93</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>94</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>9</v>
@@ -1894,43 +2080,49 @@
         <v>10</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
         <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
-        <v>95</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+        <v>121</v>
+      </c>
+      <c r="F35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>9</v>
@@ -1939,40 +2131,46 @@
         <v>10</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="E37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
-      </c>
-      <c r="E37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>110</v>
-      </c>
       <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="C38" t="s">
-        <v>95</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+      <c r="F38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>9</v>
@@ -1981,95 +2179,179 @@
         <v>10</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" t="s">
+        <v>128</v>
+      </c>
+      <c r="I44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+      <c r="C47" t="s">
         <v>114</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
         <v>94</v>
       </c>
-      <c r="C42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the firmware charicteristic have modify
</commit_message>
<xml_diff>
--- a/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
+++ b/SimpleBLEPeripheral/protocol/PGA450 profile.xlsx
@@ -370,103 +370,103 @@
     <t>0x0029</t>
   </si>
   <si>
+    <t>Transducer_Driver_Parameter</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rd Wr  0x0A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rd Wr  0x0A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    Characteristic User Description</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter 2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00:00</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 byte max</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>total 768</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">48 row </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    Simple Profile Char 6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PGA450_Parameter</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>48 row</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 byte</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notify the current row of data</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>start flag</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Transducer_Driver_Parameter</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rd Wr  0x0A</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rd Wr  0x0A</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    Characteristic User Description</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Parameter 1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Parameter 2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00:00</t>
+    <t>Row indicator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Row pointer</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>FIFO date</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 byte max</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>total 768</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FIFO row</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">48 row </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>data ready</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    Simple Profile Char 4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    Simple Profile Char 5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    Simple Profile Char 6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>PGA450_Parameter</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>48 row</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 byte</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>17 byte</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>7 byte</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>16 byte</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 byte</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notify the current row of data</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2035,7 +2035,7 @@
         <v>88</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -2052,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -2066,7 +2066,7 @@
         <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -2083,7 +2083,7 @@
         <v>96</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
@@ -2100,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
@@ -2114,10 +2114,10 @@
         <v>94</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="F35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -2134,7 +2134,7 @@
         <v>102</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
@@ -2148,7 +2148,7 @@
         <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
@@ -2162,10 +2162,10 @@
         <v>94</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -2182,7 +2182,7 @@
         <v>102</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
@@ -2193,10 +2193,10 @@
         <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -2210,10 +2210,10 @@
         <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -2230,7 +2230,7 @@
         <v>102</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
@@ -2241,7 +2241,7 @@
         <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E43" t="s">
         <v>16</v>
@@ -2255,19 +2255,19 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" t="s">
         <v>124</v>
       </c>
-      <c r="F44" t="s">
-        <v>125</v>
-      </c>
-      <c r="H44" t="s">
-        <v>128</v>
-      </c>
       <c r="I44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -2284,7 +2284,7 @@
         <v>108</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
@@ -2295,7 +2295,7 @@
         <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E46" t="s">
         <v>111</v>
@@ -2312,10 +2312,10 @@
         <v>114</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F47" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
@@ -2329,7 +2329,7 @@
         <v>94</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>